<commit_message>
Atualização 1 para os testes
</commit_message>
<xml_diff>
--- a/Firmwares/FormulaUTFPR_CAN/BUSLOAD.xlsx
+++ b/Firmwares/FormulaUTFPR_CAN/BUSLOAD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe-PC\Desktop\EK304\Firmwares\FormulaUTFPR_CAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08666212-0303-4DDF-9A76-1ADCCCEF3B76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56519858-274C-4691-A214-181534443405}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CanDB" sheetId="1" r:id="rId1"/>
@@ -1139,7 +1139,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="L24" sqref="I24:L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1970,7 +1970,7 @@
         <v>44</v>
       </c>
       <c r="L24" s="3">
-        <v>100</v>
+        <v>500</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1981,7 +1981,7 @@
       <c r="K25" s="6"/>
       <c r="L25" s="5">
         <f>J22/(L24*1000)</f>
-        <v>0.30906</v>
+        <v>6.1811999999999999E-2</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1992,7 +1992,7 @@
       <c r="K26" s="9"/>
       <c r="L26" s="5">
         <f>K22/(L24*100)</f>
-        <v>0.34920000000000001</v>
+        <v>6.9839999999999999E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2001,5 +2001,6 @@
     <mergeCell ref="I26:K26"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>